<commit_message>
updated article text, new links and resources
</commit_message>
<xml_diff>
--- a/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
+++ b/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\usr\repo\PhD_monorepo\PhD_scriptorium\article_references\2 курс\heat_and_mass_transfer\термогидродинамическое_моделирование\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DEC3E-B2E0-46ED-B2A2-1B5EB18C78BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDEF8F2-2C48-4707-9327-86AD540075F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>brief</t>
   </si>
@@ -311,12 +311,33 @@
   <si>
     <t>моделирование_течения_пластовых_флюидов\Solvent_Chamber_Development_in_3D_Model_Experiments_Vapour_Extraction_Processes_SVX.pdf</t>
   </si>
+  <si>
+    <t>Hasan A.R., Kabir C.S., “Fluid Flow and Heat Transfer in Wellbores”, SPE, Richardson, Texas, 2002</t>
+  </si>
+  <si>
+    <t>часто цитируемая книга, пока не нашел в открытом доступе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кислицын А. А. Тепломасообмен / А. А. Кислицын, А. Б. Шабаров. Тюмень: 
+изд-во ТюмГУ, 2008. </t>
+  </si>
+  <si>
+    <t>Вакулин А. А. Диагностика теплофизических параметров в нефтегазовых 
+технологиях / А. А. Вакулин, А. Б. Шабаров. Новосибирск: Наука. 
+Сиб. Издательская фирма РАН, 1998.</t>
+  </si>
+  <si>
+    <t>статьи по гидратам стр.6, 22, 50, 84, 92, 102</t>
+  </si>
+  <si>
+    <t>++'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +368,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -416,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -469,6 +497,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -750,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -764,7 +799,7 @@
     <col min="4" max="4" width="22.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.899999999999999" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" ht="16.899999999999999" x14ac:dyDescent="0.65">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -775,7 +810,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -786,7 +821,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -797,7 +832,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -808,7 +843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -817,7 +852,7 @@
       </c>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -828,7 +863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -839,7 +874,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -850,7 +885,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -859,7 +894,7 @@
       </c>
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -868,7 +903,7 @@
       </c>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -879,7 +914,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -890,7 +925,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="114" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="114" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -901,7 +936,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -912,7 +947,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="114" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="114" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -923,7 +958,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
@@ -932,6 +967,9 @@
       </c>
       <c r="C16" s="17" t="s">
         <v>68</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
@@ -1057,6 +1095,9 @@
       <c r="C27" s="9" t="s">
         <v>76</v>
       </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
@@ -1089,6 +1130,24 @@
       </c>
       <c r="C30" s="7" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="52.9" x14ac:dyDescent="0.45">
+      <c r="A31" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for overview, new articles
</commit_message>
<xml_diff>
--- a/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
+++ b/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\usr\repo\PhD_monorepo\PhD_scriptorium\article_references\2 курс\heat_and_mass_transfer\термогидродинамическое_моделирование\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDEF8F2-2C48-4707-9327-86AD540075F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DBCB85-E731-424C-BAC5-B39A1B263CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="статьи_с_обзорки" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
   <si>
     <t>brief</t>
   </si>
@@ -315,9 +326,6 @@
     <t>Hasan A.R., Kabir C.S., “Fluid Flow and Heat Transfer in Wellbores”, SPE, Richardson, Texas, 2002</t>
   </si>
   <si>
-    <t>часто цитируемая книга, пока не нашел в открытом доступе</t>
-  </si>
-  <si>
     <t xml:space="preserve">Кислицын А. А. Тепломасообмен / А. А. Кислицын, А. Б. Шабаров. Тюмень: 
 изд-во ТюмГУ, 2008. </t>
   </si>
@@ -331,13 +339,62 @@
   </si>
   <si>
     <t>++'</t>
+  </si>
+  <si>
+    <t>часто цитируемая книга, нашлел Родион Михайлович</t>
+  </si>
+  <si>
+    <t>моделирование_течения_пластовых_флюидов\Rashid_Hasan_Shah_Kabir_Fluid_Flow_and_Heat_Transfer.epub</t>
+  </si>
+  <si>
+    <t>шагаипов особенности выпадения гидратов в стоячей воде</t>
+  </si>
+  <si>
+    <t>Особенности процесса образования гидратных частиц в стоячей воде</t>
+  </si>
+  <si>
+    <t>Вестник_Тюмгу\Shagaipow_features_of_hydate_particles_formation_in_still_water.pdf</t>
+  </si>
+  <si>
+    <t>Выпуски</t>
+  </si>
+  <si>
+    <t>https://vestnik.utmn.ru/energy/vypuski/</t>
+  </si>
+  <si>
+    <t>Определение глубины 
+газогидратообразования в нефтяных 
+скважинах с учетом режима ее работы 
+и состава попутного газа</t>
+  </si>
+  <si>
+    <t>Вестник_Тюмгу\molchnova_determine_the_depth_of_gas_hydrate_formations.pdf</t>
+  </si>
+  <si>
+    <t>Вестник_Тюмгу\Shagaipov_the_induction_period_of_hydrate_formation_in_contact_gas_and_water.pdf</t>
+  </si>
+  <si>
+    <t>юя $ 8 7</t>
+  </si>
+  <si>
+    <t>© В. Ш. ШАГАПОВ, А. В. ЯЛАЕВ, О. А. ШЕПЕЛЬКЕВИЧ 
+Период индукции гидратообразования при контакте газа и воды</t>
+  </si>
+  <si>
+    <t>Описание гидродинамических и температурных полей при разработке газогидратных пластов</t>
+  </si>
+  <si>
+    <t>юя 5 A B = 8 :</t>
+  </si>
+  <si>
+    <t>Вестник_Тюмгу\Шагапов_описание_гидродинамических_и_температурных_полей_при_разработке_газогидратных_пластов.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +432,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="FiraSans-Regular"/>
     </font>
   </fonts>
   <fills count="5">
@@ -444,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +566,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -785,21 +867,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="37.46484375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.73046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.73046875" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.899999999999999" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="16.899999999999999">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -810,7 +890,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="71.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -820,8 +900,11 @@
       <c r="C2" s="15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="57">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -832,7 +915,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="57">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -843,7 +926,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="28.5">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -852,7 +935,7 @@
       </c>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="85.5">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -863,7 +946,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="85.5">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -874,7 +957,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="57">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -885,7 +968,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="57">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -894,7 +977,7 @@
       </c>
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="42.75">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -903,7 +986,7 @@
       </c>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="42.75">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -914,7 +997,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="71.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -925,7 +1008,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="114">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -936,7 +1019,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="71.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -947,7 +1030,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="114">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -958,7 +1041,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="57">
       <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
@@ -969,10 +1052,10 @@
         <v>68</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="71.25">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
@@ -983,7 +1066,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="71.25">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -994,7 +1077,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="156.75">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -1005,7 +1088,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="142.5">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -1016,7 +1099,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="85.5">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1027,7 +1110,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="71.25">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
@@ -1038,7 +1121,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="99.75">
       <c r="A23" s="4" t="s">
         <v>30</v>
       </c>
@@ -1049,7 +1132,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="99.75">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
@@ -1060,7 +1143,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="42.75">
       <c r="A25" s="11" t="s">
         <v>49</v>
       </c>
@@ -1071,7 +1154,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="57">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
@@ -1085,7 +1168,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="42.75">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
@@ -1096,10 +1179,10 @@
         <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="42.75">
       <c r="A28" s="13" t="s">
         <v>53</v>
       </c>
@@ -1110,7 +1193,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="42.75">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -1121,7 +1204,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="71.25">
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
@@ -1132,22 +1215,71 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="52.9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="52.9">
       <c r="A31" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="42.75">
+      <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" ht="85.5">
+      <c r="A33" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>89</v>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" ht="57">
+      <c r="A34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="57">
+      <c r="A35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="57">
+      <c r="A36" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="71.25">
+      <c r="A37" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1200,8 +1332,240 @@
     <hyperlink ref="B30" r:id="rId46" display="https://www.researchgate.net/publication/349714239_Blastomilonitovye_kompleksy_zapadnoj_casti_Enisejskogo_kraza_Vostocnaa_Sibir_Rossia_geologiceskaa_pozicia_evolucia_metamorfizma_i_geodinamiceskie_modeli" xr:uid="{BC784919-0BD7-442A-AD5E-A02C2F8EA24A}"/>
     <hyperlink ref="C30" r:id="rId47" xr:uid="{9D248054-356E-465F-A828-EC17EE90ED54}"/>
     <hyperlink ref="C24" r:id="rId48" xr:uid="{D1E8A270-EE9D-482D-B216-82FDE092E521}"/>
+    <hyperlink ref="C31" r:id="rId49" xr:uid="{F30B1F7E-5858-427E-B411-440299490ADA}"/>
+    <hyperlink ref="B34" r:id="rId50" display="https://vestnik.utmn.ru/energy/vypuski/2015-tom-1/2-2/113210/?ysclid=m5toljgtnc639660816" xr:uid="{C492C9B8-A25A-4DC7-96F5-153065B1F8E9}"/>
+    <hyperlink ref="C34" r:id="rId51" xr:uid="{2EE39A59-302E-413D-B61F-4910A6C83386}"/>
+    <hyperlink ref="B35" r:id="rId52" display="https://vestnik.utmn.ru/energy/vypuski/" xr:uid="{3C791538-492A-457D-B7DD-D35A7F00CCD2}"/>
+    <hyperlink ref="C35" r:id="rId53" xr:uid="{906F82C3-3A28-4B47-9FCA-39E905E69DE9}"/>
+    <hyperlink ref="C36" r:id="rId54" xr:uid="{0922951F-DABA-48B2-ABE4-52BADBE2F0BB}"/>
+    <hyperlink ref="B36" r:id="rId55" display="https://vestnik.utmn.ru/upload/iblock/b90/6_%D0%92. %D0%A8. %D0%A8%D0%B0%D0%B3%D0%B0%D0%BF%D0%BE%D0%B2, %D0%90. %D0%92. %D0%AF%D0%BB%D0%B0%D0%B5%D0%B2, %D0%9E. %D0%90. %D0%A8%D0%B5%D0%BF%D0%B5%D0%BB%D1%8C%D0%BA%D0%B5%D0%B2%D0%B8%D1%87.pdf" xr:uid="{FEE975BF-3DB3-41CE-A295-047F59186DB1}"/>
+    <hyperlink ref="B37" r:id="rId56" display="https://vestnik.utmn.ru/upload/iblock/7ed/%D0%A8%D0%B0%D0%B3%D0%B0%D0%BF%D0%BE%D0%B2_%D0%A7%D0%B8%D0%B3%D0%BB%D0%B8%D0%BD%D1%86%D0%B5%D0%B2%D0%B0_%D0%A0%D1%83%D1%81%D0%B8%D0%BD%D0%BE%D0%B2.pdf" xr:uid="{4BBC2C49-536C-442E-AD47-4ED322495F56}"/>
+    <hyperlink ref="C37" r:id="rId57" xr:uid="{58343CCE-BD69-4A31-8E9A-0D1D6D5F4290}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AAEED9-6B5E-406E-A324-B6384A2BB2F5}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="48.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="16">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="16">
+        <f>A1+1</f>
+        <v>2</v>
+      </c>
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="16">
+        <f t="shared" ref="A3:A27" si="0">A2+1</f>
+        <v>3</v>
+      </c>
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="1:2" ht="28.5">
+      <c r="A4" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.5">
+      <c r="A5" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="24"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="24"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="24"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="24"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="24"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="24"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="24"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="16">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="16">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="24"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="24"/>
+    </row>
+    <row r="21" spans="1:2" ht="28.5">
+      <c r="A21" s="16">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.5">
+      <c r="A22" s="16">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="28.5">
+      <c r="A23" s="16">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="42.75">
+      <c r="A24" s="16">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="16">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="16">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{8D8062B0-5D3F-451B-AAC7-4903EB34D031}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{8F314E71-BF3B-4E5E-ACF2-A6268B27AB29}"/>
+    <hyperlink ref="B21" r:id="rId3" xr:uid="{8BB9C8AC-6975-4865-9B5D-5E8ABACF5A2E}"/>
+    <hyperlink ref="B22" r:id="rId4" xr:uid="{60F1D140-5D01-4DA2-90E3-BE89338963E7}"/>
+    <hyperlink ref="B23" r:id="rId5" xr:uid="{C9F909C5-1E56-4312-A76B-F6E4FD6E3958}"/>
+    <hyperlink ref="B24" r:id="rId6" xr:uid="{D947E291-2033-435F-9DCB-40495FC19B9B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to article and reference files
</commit_message>
<xml_diff>
--- a/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
+++ b/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\usr\repo\PhD_monorepo\PhD_scriptorium\article_references\2 курс\heat_and_mass_transfer\термогидродинамическое_моделирование\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DBCB85-E731-424C-BAC5-B39A1B263CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38932EB1-F3CA-426F-8F5F-1E2BD6576F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="статьи_с_обзорки" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>brief</t>
   </si>
@@ -506,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,6 +584,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -869,7 +871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -1194,7 +1198,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="42.75">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1351,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AAEED9-6B5E-406E-A324-B6384A2BB2F5}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1364,7 +1368,9 @@
       <c r="A1" s="16">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="29" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="16">
@@ -1565,6 +1571,7 @@
     <hyperlink ref="B22" r:id="rId4" xr:uid="{60F1D140-5D01-4DA2-90E3-BE89338963E7}"/>
     <hyperlink ref="B23" r:id="rId5" xr:uid="{C9F909C5-1E56-4312-A76B-F6E4FD6E3958}"/>
     <hyperlink ref="B24" r:id="rId6" xr:uid="{D947E291-2033-435F-9DCB-40495FC19B9B}"/>
+    <hyperlink ref="B1" r:id="rId7" xr:uid="{8EB13256-BC1C-4442-99BB-C8399F6E1DFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update in links and article text
</commit_message>
<xml_diff>
--- a/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
+++ b/article_references/2 курс/heat_and_mass_transfer/термогидродинамическое_моделирование/ссылки.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\usr\repo\PhD_monorepo\PhD_scriptorium\article_references\2 курс\heat_and_mass_transfer\термогидродинамическое_моделирование\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38932EB1-F3CA-426F-8F5F-1E2BD6576F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1291F4-CF90-4A7E-8AF2-A63390981D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
   <si>
     <t>brief</t>
   </si>
@@ -387,6 +387,42 @@
   </si>
   <si>
     <t>Вестник_Тюмгу\Шагапов_описание_гидродинамических_и_температурных_полей_при_разработке_газогидратных_пластов.pdf</t>
+  </si>
+  <si>
+    <t>обзор модулей tNavigator</t>
+  </si>
+  <si>
+    <t>tnav-modules-booklet-2022-ru.pdf</t>
+  </si>
+  <si>
+    <t>гидраты_моделирование_температуры\RFD_Термические_модели.pdf</t>
+  </si>
+  <si>
+    <t>работа с термическими моделями</t>
+  </si>
+  <si>
+    <t>РФД_навигатор\tnav-modules-booklet-2022-ru.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.petroleumengineers.ru/node/4325?ysclid=m64kf5hju5925364188 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">проблемы при моделировании нагнетании пара </t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>517 страница допущения для фазового равновесия мануал RFD</t>
+  </si>
+  <si>
+    <t>обзор моделей и численных методовm, на основе которых работают симуляторы</t>
+  </si>
+  <si>
+    <t>http://proceedings.socar.az</t>
+  </si>
+  <si>
+    <t>моделирование_течения_пластовых_флюидов\SOCAR_simulators_120_130_OGP20230300894.pdf</t>
   </si>
 </sst>
 </file>
@@ -505,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,6 +623,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -869,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1284,6 +1325,44 @@
       </c>
       <c r="C37" s="7" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="42.75">
+      <c r="A38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="42.75">
+      <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="28.9">
+      <c r="A40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="57">
+      <c r="A41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1345,23 +1424,28 @@
     <hyperlink ref="B36" r:id="rId55" display="https://vestnik.utmn.ru/upload/iblock/b90/6_%D0%92. %D0%A8. %D0%A8%D0%B0%D0%B3%D0%B0%D0%BF%D0%BE%D0%B2, %D0%90. %D0%92. %D0%AF%D0%BB%D0%B0%D0%B5%D0%B2, %D0%9E. %D0%90. %D0%A8%D0%B5%D0%BF%D0%B5%D0%BB%D1%8C%D0%BA%D0%B5%D0%B2%D0%B8%D1%87.pdf" xr:uid="{FEE975BF-3DB3-41CE-A295-047F59186DB1}"/>
     <hyperlink ref="B37" r:id="rId56" display="https://vestnik.utmn.ru/upload/iblock/7ed/%D0%A8%D0%B0%D0%B3%D0%B0%D0%BF%D0%BE%D0%B2_%D0%A7%D0%B8%D0%B3%D0%BB%D0%B8%D0%BD%D1%86%D0%B5%D0%B2%D0%B0_%D0%A0%D1%83%D1%81%D0%B8%D0%BD%D0%BE%D0%B2.pdf" xr:uid="{4BBC2C49-536C-442E-AD47-4ED322495F56}"/>
     <hyperlink ref="C37" r:id="rId57" xr:uid="{58343CCE-BD69-4A31-8E9A-0D1D6D5F4290}"/>
+    <hyperlink ref="B38" r:id="rId58" display="https://www.ipng.ru/scientific-activity/academic/tnav-modules-booklet-2022-ru.pdf" xr:uid="{7AEF665F-49AD-452F-8606-68EF43F9192F}"/>
+    <hyperlink ref="C39" r:id="rId59" xr:uid="{B5B76BF9-C497-41FC-8462-9C0218D38BCE}"/>
+    <hyperlink ref="C38" r:id="rId60" xr:uid="{764BEA22-2491-4BEA-940E-98A6C23D3035}"/>
+    <hyperlink ref="C41" r:id="rId61" xr:uid="{0A01FDB3-0A51-48AE-9E7D-37DD613501CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AAEED9-6B5E-406E-A324-B6384A2BB2F5}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="48.86328125" customWidth="1"/>
+    <col min="3" max="3" width="31.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1481,35 +1565,35 @@
       </c>
       <c r="B16" s="24"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B17" s="24"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B18" s="24"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B19" s="24"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B20" s="24"/>
     </row>
-    <row r="21" spans="1:2" ht="28.5">
+    <row r="21" spans="1:3" ht="28.5">
       <c r="A21" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1518,7 +1602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="28.5">
+    <row r="22" spans="1:3" ht="28.5">
       <c r="A22" s="16">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1527,7 +1611,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="28.5">
+    <row r="23" spans="1:3" ht="28.5">
       <c r="A23" s="16">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1536,7 +1620,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:3" ht="42.75">
       <c r="A24" s="16">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1545,22 +1629,39 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:3" ht="34.5" customHeight="1">
       <c r="A25" s="16">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="16">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="B26" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="16">
         <f t="shared" si="0"/>
         <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.5">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1572,6 +1673,9 @@
     <hyperlink ref="B23" r:id="rId5" xr:uid="{C9F909C5-1E56-4312-A76B-F6E4FD6E3958}"/>
     <hyperlink ref="B24" r:id="rId6" xr:uid="{D947E291-2033-435F-9DCB-40495FC19B9B}"/>
     <hyperlink ref="B1" r:id="rId7" xr:uid="{8EB13256-BC1C-4442-99BB-C8399F6E1DFB}"/>
+    <hyperlink ref="C25" r:id="rId8" xr:uid="{1968792E-B1D7-411C-9285-CD2B2E9ED878}"/>
+    <hyperlink ref="B25" r:id="rId9" xr:uid="{37E13587-380E-410C-A689-022C23EA0478}"/>
+    <hyperlink ref="B26" r:id="rId10" xr:uid="{251107CF-B044-4D7E-ACE8-DFC9A65BD0DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>